<commit_message>
added some result tables for report
</commit_message>
<xml_diff>
--- a/20 Results/codonsunderselection.xlsx
+++ b/20 Results/codonsunderselection.xlsx
@@ -134,8 +134,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -187,35 +187,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -501,7 +501,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,45 +509,45 @@
     <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -561,10 +561,10 @@
       <c r="C3" s="1">
         <v>24</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>0.10863399999999999</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>0.91405999999999998</v>
       </c>
     </row>
@@ -575,10 +575,10 @@
       <c r="C4" s="1">
         <v>27</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>9.5940999999999999E-2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>0.95108899999999996</v>
       </c>
     </row>
@@ -589,10 +589,10 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>8.7508799999999998E-2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>0.932091</v>
       </c>
     </row>
@@ -600,62 +600,62 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>12</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>0.35686400000000001</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>0.98617500000000002</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="7">
         <v>1.0442400000000001</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="9">
         <v>2.43019E-3</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>96</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>0.16140699999999999</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>0.967839</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="7">
         <v>0.50683400000000001</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="9">
         <v>7.1484599999999997E-3</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="6">
         <v>5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>7.3642799999999994E-2</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>0.98506400000000005</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>96.14</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="9">
         <v>1.2946999999999999E-4</v>
       </c>
     </row>
@@ -663,17 +663,23 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="6">
         <v>170</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="7">
         <v>0.66186999999999996</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="7">
         <v>0.92744800000000005</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1.9673700000000001</v>
+      </c>
+      <c r="G9" s="9">
+        <v>4.7283899999999997E-2</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -683,33 +689,33 @@
       <c r="C10" s="1">
         <v>127</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>0.23341000000000001</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>0.91909200000000002</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -736,41 +742,41 @@
   <cols>
     <col min="1" max="1" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -778,19 +784,19 @@
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <v>0.32226700000000003</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>0.99858100000000005</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="8">
         <v>39.451900000000002</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="9">
         <v>4.4408900000000002E-16</v>
       </c>
     </row>
@@ -798,28 +804,28 @@
       <c r="B4" s="1">
         <v>161</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>0.19864299999999999</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>0.919076</v>
       </c>
       <c r="E4">
         <v>1.4898199999999999</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>0.13706299999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
updated results for reporting
</commit_message>
<xml_diff>
--- a/20 Results/codonsunderselection.xlsx
+++ b/20 Results/codonsunderselection.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qx217\Documents\rotavirus\20 Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rotavirus\20 Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Proteins" sheetId="1" r:id="rId1"/>
     <sheet name="Vaccine" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Dataset</t>
   </si>
@@ -103,8 +103,17 @@
     <t>P.Pr.</t>
   </si>
   <si>
+    <t>Table 4: Genes under Diversifying Selection</t>
+  </si>
+  <si>
+    <t>2*</t>
+  </si>
+  <si>
+    <t>Table 5: Genes under Diversifying Selection after the  Introduction of Modern Vaccines</t>
+  </si>
+  <si>
     <r>
-      <t>The number of sequences accepted by HyPhy for analysis is shown by "n". "β-α" is the difference between synonymous (α) and non-synonymous (β) substitution rates over sites. "P.Pr." is the posterior probability of positive selection. "β</t>
+      <t>The number of sequences accepted by HyPhy for analysis is shown by "n". "β-α" is the difference between synonymous (α) and non-synonymous (β) substitution rates over sites and a positive value denotes diversifying selection. "P.Pr." is the posterior probability of positive selection. "β</t>
     </r>
     <r>
       <rPr>
@@ -125,19 +134,46 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">" is the unconstrained estimate for the non-synonymous rate in MEME. Sites found under positive selection by both FUBAR and MEME were bolded. </t>
+      <t xml:space="preserve">" is the unconstrained estimate for the non-synonymous rate in MEME. All listed proteins were found under pervasive and episodic positive selection by both FUBAR and MEME. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The number of sequences accepted by HyPhy for analysis is shown by "n". "β-α" is the difference between synonymous (α) and non-synonymous (β) substitution rates over sites and a positive value denotes diversifying selection."P.Pr." is the posterior probability of positive selection. "β</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" is the unconstrained estimate for the non-synonymous rate in MEME. 
+*Only codon 2 was found under pervasive and episodic positive selection by both FUBAR and MEME.</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,16 +197,314 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -178,18 +512,243 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -199,28 +758,140 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -311,6 +982,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -346,6 +1034,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,233 +1205,277 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="13">
         <v>24</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D4" s="14">
         <v>0.10863399999999999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E4" s="14">
         <v>0.91405999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="14">
+        <v>1.64489</v>
+      </c>
+      <c r="G4" s="15">
+        <v>2.3427199999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="13">
         <v>27</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="14">
         <v>9.5940999999999999E-2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E5" s="14">
         <v>0.95108899999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="F5" s="14">
+        <v>0.33221800000000001</v>
+      </c>
+      <c r="G5" s="15">
+        <v>2.2234E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="13">
         <v>2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D6" s="14">
         <v>8.7508799999999998E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E6" s="14">
         <v>0.932091</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="F6" s="14">
+        <v>50.200099999999999</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1.77645E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C7" s="13">
         <v>12</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D7" s="14">
         <v>0.35686400000000001</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E7" s="14">
         <v>0.98617500000000002</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F7" s="14">
         <v>1.0442400000000001</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G7" s="15">
         <v>2.43019E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C8" s="13">
         <v>96</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="14">
         <v>0.16140699999999999</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="14">
         <v>0.967839</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F8" s="14">
         <v>0.50683400000000001</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G8" s="15">
         <v>7.1484599999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C9" s="13">
         <v>5</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D9" s="14">
         <v>7.3642799999999994E-2</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E9" s="14">
         <v>0.98506400000000005</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F9" s="14">
         <v>96.14</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G9" s="15">
         <v>1.2946999999999999E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C10" s="13">
         <v>170</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="14">
         <v>0.66186999999999996</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E10" s="14">
         <v>0.92744800000000005</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="14">
         <v>1.9673700000000001</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G10" s="15">
         <v>4.7283899999999997E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="31"/>
+      <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="16">
         <v>127</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="17">
         <v>0.23341000000000001</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E11" s="17">
         <v>0.91909200000000002</v>
       </c>
+      <c r="F11" s="17">
+        <v>11.3208</v>
+      </c>
+      <c r="G11" s="18">
+        <v>1.4050099999999999E-4</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="A12" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A12:G12"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -734,107 +1483,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="10.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="10">
         <v>0.32226700000000003</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D4" s="10">
         <v>0.99858100000000005</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E4" s="9">
         <v>39.451900000000002</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F4" s="11">
         <v>4.4408900000000002E-16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34"/>
+      <c r="B5" s="5">
         <v>161</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="20">
         <v>0.19864299999999999</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="20">
         <v>0.919076</v>
       </c>
-      <c r="E4">
+      <c r="E5" s="5">
         <v>1.4898199999999999</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F5" s="21">
         <v>0.13706299999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+    <row r="6" spans="1:6" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
+  <mergeCells count="7">
     <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated annotations for data tables
</commit_message>
<xml_diff>
--- a/20 Results/codonsunderselection.xlsx
+++ b/20 Results/codonsunderselection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rotavirus\20 Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qx217\Documents\rotavirus\20 Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Proteins" sheetId="1" r:id="rId1"/>
     <sheet name="Vaccine" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,17 +103,17 @@
     <t>P.Pr.</t>
   </si>
   <si>
-    <t>Table 4: Genes under Diversifying Selection</t>
-  </si>
-  <si>
     <t>2*</t>
   </si>
   <si>
-    <t>Table 5: Genes under Diversifying Selection after the  Introduction of Modern Vaccines</t>
+    <t>Table 4: Sites under Diversifying Selection</t>
+  </si>
+  <si>
+    <t>Table 5: Sites under Diversifying Selection after the Introduction of Modern Vaccines</t>
   </si>
   <si>
     <r>
-      <t>The number of sequences accepted by HyPhy for analysis is shown by "n". "β-α" is the difference between synonymous (α) and non-synonymous (β) substitution rates over sites and a positive value denotes diversifying selection. "P.Pr." is the posterior probability of positive selection. "β</t>
+      <t>The number of sequences accepted by HyPhy for analysis is shown by "n". "β-α" is the difference between synonymous (α) and non-synonymous (β) substitution rates over sites and a positive value denotes diversifying selection. "P.Pr." is the posterior probability of diversifying selection. "β</t>
     </r>
     <r>
       <rPr>
@@ -134,12 +134,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">" is the unconstrained estimate for the non-synonymous rate in MEME. All listed proteins were found under pervasive and episodic positive selection by both FUBAR and MEME. </t>
+      <t xml:space="preserve">" is the unconstrained estimate for the non-synonymous rate in MEME. All listed proteins were found under both pervasive and episodic diversifying selection by FUBAR (P.Pr.&gt;0.9) and MEME (p-value&lt;0.1) respectively. </t>
     </r>
   </si>
   <si>
     <r>
-      <t>The number of sequences accepted by HyPhy for analysis is shown by "n". "β-α" is the difference between synonymous (α) and non-synonymous (β) substitution rates over sites and a positive value denotes diversifying selection."P.Pr." is the posterior probability of positive selection. "β</t>
+      <t>The number of sequences accepted by HyPhy for analysis is shown by "n". "β-α" is the difference between synonymous (α) and non-synonymous (β) substitution rates over sites and a positive value denotes diversifying selection."P.Pr." is the posterior probability of diversifying selection. "β</t>
     </r>
     <r>
       <rPr>
@@ -161,14 +161,14 @@
         <scheme val="minor"/>
       </rPr>
       <t>" is the unconstrained estimate for the non-synonymous rate in MEME. 
-*Only codon 2 was found under pervasive and episodic positive selection by both FUBAR and MEME.</t>
+*Only codon 2 was found under both pervasive and episodic diversifying selection by FUBAR (P.Pr.&gt;0.9) and MEME (p-value&lt;0.1) respectively. Codon 161 was found under pervasive diversifying selection by FUBAR (P.Pr.&gt;0.9) but not detected for episodic positive selection by MEME (p-value&gt;0.1).</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
@@ -839,14 +839,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -982,23 +982,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1034,23 +1017,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1206,7 +1172,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G12"/>
+      <selection sqref="A1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1187,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -1484,7 +1450,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,14 +1463,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -1539,11 +1505,11 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="10">
         <v>0.32226700000000003</v>
@@ -1559,7 +1525,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="5">
         <v>161</v>
       </c>

</xml_diff>